<commit_message>
Completed linear regression with adjusted r-squared and RMSE
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\my_stuff\development\python\ddw\2d_mulitple_linear_regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{323E9D82-5881-40B5-B606-431F48D0588D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2186264-9DED-4257-8692-9AF4D979A389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="2910" windowWidth="16200" windowHeight="9848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="122">
   <si>
     <t>Country</t>
   </si>
@@ -399,6 +399,9 @@
   </si>
   <si>
     <t>Global Food Security Index 2020 (GFSI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -818,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F108" sqref="F108"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3359,8 +3362,8 @@
       <c r="F110" s="4">
         <v>44.3</v>
       </c>
-      <c r="G110" s="4">
-        <v>320.27182420000003</v>
+      <c r="G110" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.45">
@@ -3457,5 +3460,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed annotations, added comparison for minmax normalization
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\my_stuff\development\python\ddw\2d_mulitple_linear_regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2186264-9DED-4257-8692-9AF4D979A389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCCB423-B2C5-4FE6-AB2E-48ECE117CEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -831,9 +831,9 @@
     <col min="2" max="2" width="13.3984375" style="11" customWidth="1"/>
     <col min="3" max="3" width="12.06640625" style="6" customWidth="1"/>
     <col min="4" max="4" width="10.59765625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.265625" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.3984375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.06640625" style="5"/>
+    <col min="7" max="7" width="28.19921875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="57" x14ac:dyDescent="0.45">

</xml_diff>